<commit_message>
update data filename and fix bug on matlab code
</commit_message>
<xml_diff>
--- a/Data/Data_detail.xlsx
+++ b/Data/Data_detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester3\ML-AIS\ML-AIS-Sensor-Project-2021\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB5BB2C-32A7-4D29-AC41-64A89F475775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95652B02-823B-4ACE-922A-A7E4DC16143A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="712" firstSheet="3" activeTab="3" xr2:uid="{3488F8F7-C072-46D5-A2BC-EFBC329B43B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="712" firstSheet="3" activeTab="7" xr2:uid="{3488F8F7-C072-46D5-A2BC-EFBC329B43B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="7" state="hidden" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10864" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10872" uniqueCount="246">
   <si>
     <t>No.</t>
   </si>
@@ -50891,7 +50891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19791E42-7636-4F38-95C8-773C092ADBC2}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -68373,7 +68373,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9383A25-0F16-46DD-90D6-054193614933}">
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74:H81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -70672,9 +70674,8 @@
         <f t="shared" si="11"/>
         <v>250</v>
       </c>
-      <c r="H74" s="90" t="str">
-        <f t="shared" si="10"/>
-        <v>fft_73_.txt</v>
+      <c r="H74" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="I74" s="80" t="s">
         <v>18</v>
@@ -70703,9 +70704,8 @@
         <f t="shared" si="11"/>
         <v>250</v>
       </c>
-      <c r="H75" s="90" t="str">
-        <f>_xlfn.CONCAT("fft_",A75,"_",".txt")</f>
-        <v>fft_74_.txt</v>
+      <c r="H75" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="I75" s="80" t="s">
         <v>18</v>
@@ -70734,9 +70734,8 @@
         <f t="shared" si="11"/>
         <v>250</v>
       </c>
-      <c r="H76" s="90" t="str">
-        <f t="shared" ref="H76:H105" si="12">_xlfn.CONCAT("fft_",A76,"_",".txt")</f>
-        <v>fft_75_.txt</v>
+      <c r="H76" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="I76" s="80" t="s">
         <v>18</v>
@@ -70765,9 +70764,8 @@
         <f t="shared" si="11"/>
         <v>250</v>
       </c>
-      <c r="H77" s="90" t="str">
-        <f t="shared" si="12"/>
-        <v>fft_76_.txt</v>
+      <c r="H77" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="I77" s="80" t="s">
         <v>18</v>
@@ -70796,9 +70794,8 @@
         <f t="shared" si="11"/>
         <v>250</v>
       </c>
-      <c r="H78" s="90" t="str">
-        <f t="shared" si="12"/>
-        <v>fft_77_.txt</v>
+      <c r="H78" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="I78" s="80" t="s">
         <v>18</v>
@@ -70827,9 +70824,8 @@
         <f t="shared" si="11"/>
         <v>250</v>
       </c>
-      <c r="H79" s="90" t="str">
-        <f t="shared" si="12"/>
-        <v>fft_78_.txt</v>
+      <c r="H79" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="I79" s="80" t="s">
         <v>18</v>
@@ -70858,9 +70854,8 @@
         <f>F80*10</f>
         <v>250</v>
       </c>
-      <c r="H80" s="90" t="str">
-        <f t="shared" si="12"/>
-        <v>fft_79_.txt</v>
+      <c r="H80" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="I80" s="80" t="s">
         <v>18</v>
@@ -70886,12 +70881,11 @@
         <v>25</v>
       </c>
       <c r="G81" s="82">
-        <f t="shared" ref="G81" si="13">F81*10</f>
+        <f t="shared" ref="G81" si="12">F81*10</f>
         <v>250</v>
       </c>
-      <c r="H81" s="90" t="str">
-        <f t="shared" si="12"/>
-        <v>fft_80_.txt</v>
+      <c r="H81" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="I81" s="80" t="s">
         <v>18</v>
@@ -70921,7 +70915,7 @@
         <v>400</v>
       </c>
       <c r="H82" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="H76:H105" si="13">_xlfn.CONCAT("fft_",A82,"_",".txt")</f>
         <v>fft_81_.txt</v>
       </c>
       <c r="I82" s="80" t="s">
@@ -70952,7 +70946,7 @@
         <v>400</v>
       </c>
       <c r="H83" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_82_.txt</v>
       </c>
       <c r="I83" s="80" t="s">
@@ -70983,7 +70977,7 @@
         <v>400</v>
       </c>
       <c r="H84" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_83_.txt</v>
       </c>
       <c r="I84" s="80" t="s">
@@ -71014,7 +71008,7 @@
         <v>400</v>
       </c>
       <c r="H85" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_84_.txt</v>
       </c>
       <c r="I85" s="80" t="s">
@@ -71045,7 +71039,7 @@
         <v>400</v>
       </c>
       <c r="H86" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_85_.txt</v>
       </c>
       <c r="I86" s="80" t="s">
@@ -71076,7 +71070,7 @@
         <v>400</v>
       </c>
       <c r="H87" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_86_.txt</v>
       </c>
       <c r="I87" s="80" t="s">
@@ -71107,7 +71101,7 @@
         <v>400</v>
       </c>
       <c r="H88" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_87_.txt</v>
       </c>
       <c r="I88" s="80" t="s">
@@ -71138,7 +71132,7 @@
         <v>400</v>
       </c>
       <c r="H89" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_88_.txt</v>
       </c>
       <c r="I89" s="80" t="s">
@@ -71169,7 +71163,7 @@
         <v>400</v>
       </c>
       <c r="H90" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_89_.txt</v>
       </c>
       <c r="I90" s="80" t="s">
@@ -71200,7 +71194,7 @@
         <v>400</v>
       </c>
       <c r="H91" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_90_.txt</v>
       </c>
       <c r="I91" s="80" t="s">
@@ -71231,7 +71225,7 @@
         <v>400</v>
       </c>
       <c r="H92" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_91_.txt</v>
       </c>
       <c r="I92" s="80" t="s">
@@ -71262,7 +71256,7 @@
         <v>400</v>
       </c>
       <c r="H93" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_92_.txt</v>
       </c>
       <c r="I93" s="80" t="s">
@@ -71293,7 +71287,7 @@
         <v>400</v>
       </c>
       <c r="H94" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_93_.txt</v>
       </c>
       <c r="I94" s="80" t="s">
@@ -71324,7 +71318,7 @@
         <v>400</v>
       </c>
       <c r="H95" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_94_.txt</v>
       </c>
       <c r="I95" s="80" t="s">
@@ -71355,7 +71349,7 @@
         <v>400</v>
       </c>
       <c r="H96" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_95_.txt</v>
       </c>
       <c r="I96" s="80" t="s">
@@ -71386,7 +71380,7 @@
         <v>400</v>
       </c>
       <c r="H97" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_96_.txt</v>
       </c>
       <c r="I97" s="80" t="s">
@@ -71417,7 +71411,7 @@
         <v>400</v>
       </c>
       <c r="H98" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_97_.txt</v>
       </c>
       <c r="I98" s="80" t="s">
@@ -71448,7 +71442,7 @@
         <v>400</v>
       </c>
       <c r="H99" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_98_.txt</v>
       </c>
       <c r="I99" s="80" t="s">
@@ -71510,7 +71504,7 @@
         <v>400</v>
       </c>
       <c r="H101" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_100_.txt</v>
       </c>
       <c r="I101" s="80" t="s">
@@ -71541,7 +71535,7 @@
         <v>400</v>
       </c>
       <c r="H102" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_101_.txt</v>
       </c>
       <c r="I102" s="80" t="s">
@@ -71572,7 +71566,7 @@
         <v>400</v>
       </c>
       <c r="H103" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_102_.txt</v>
       </c>
       <c r="I103" s="80" t="s">
@@ -71603,7 +71597,7 @@
         <v>400</v>
       </c>
       <c r="H104" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_103_.txt</v>
       </c>
       <c r="I104" s="80" t="s">
@@ -71634,7 +71628,7 @@
         <v>400</v>
       </c>
       <c r="H105" s="90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>fft_104_.txt</v>
       </c>
       <c r="I105" s="80" t="s">
@@ -72403,7 +72397,7 @@
       </c>
       <c r="H130" s="87">
         <f>COUNTIF($H$2:$H129, "fft*")</f>
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="I130" s="26" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
fix bug in program ( still have bug on filter -> movement not working ) and push evaluation result to branch
</commit_message>
<xml_diff>
--- a/Data/Data_detail.xlsx
+++ b/Data/Data_detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester3\ML-AIS\ML-AIS-Sensor-Project-2021\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95652B02-823B-4ACE-922A-A7E4DC16143A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65DC73F-3027-4749-9CAF-E80BA7A6CA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="712" firstSheet="3" activeTab="7" xr2:uid="{3488F8F7-C072-46D5-A2BC-EFBC329B43B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="712" firstSheet="6" activeTab="8" xr2:uid="{3488F8F7-C072-46D5-A2BC-EFBC329B43B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="7" state="hidden" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10872" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10560" uniqueCount="246">
   <si>
     <t>No.</t>
   </si>
@@ -12407,7 +12407,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2538E6AB-C645-4E96-A765-27DC877B237F}">
-  <dimension ref="A1:K162"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -16147,7 +16147,7 @@
         <v>40</v>
       </c>
       <c r="I101" s="1">
-        <f t="shared" ref="I101:I115" si="13">H101*10</f>
+        <f t="shared" ref="I101:I109" si="13">H101*10</f>
         <v>400</v>
       </c>
       <c r="J101" s="1" t="s">
@@ -16449,1913 +16449,41 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="15" customHeight="1">
-      <c r="A110" s="80">
-        <v>109</v>
-      </c>
-      <c r="B110" s="100">
-        <v>180</v>
-      </c>
-      <c r="C110" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D110" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E110" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F110" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H110" s="1">
-        <v>40</v>
+    <row r="110" spans="1:11">
+      <c r="A110" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B110" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="C110" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="D110" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="E110" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="F110" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="G110" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="H110" s="99">
+        <f>SUM(H2:H109)</f>
+        <v>4320</v>
       </c>
       <c r="I110" s="1">
-        <f t="shared" si="13"/>
-        <v>400</v>
-      </c>
-      <c r="J110" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K110" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" ht="15" customHeight="1">
-      <c r="A111" s="80">
-        <v>110</v>
-      </c>
-      <c r="B111" s="100">
-        <v>180</v>
-      </c>
-      <c r="C111" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D111" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E111" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F111" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H111" s="1">
-        <v>40</v>
-      </c>
-      <c r="I111" s="1">
-        <f t="shared" si="13"/>
-        <v>400</v>
-      </c>
-      <c r="J111" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K111" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" ht="15" customHeight="1">
-      <c r="A112" s="80">
-        <v>111</v>
-      </c>
-      <c r="B112" s="100">
-        <v>180</v>
-      </c>
-      <c r="C112" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D112" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E112" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F112" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H112" s="1">
-        <v>40</v>
-      </c>
-      <c r="I112" s="1">
-        <f t="shared" si="13"/>
-        <v>400</v>
-      </c>
-      <c r="J112" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K112" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" ht="15" customHeight="1">
-      <c r="A113" s="80">
-        <v>112</v>
-      </c>
-      <c r="B113" s="100">
-        <v>180</v>
-      </c>
-      <c r="C113" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D113" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E113" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F113" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H113" s="1">
-        <v>40</v>
-      </c>
-      <c r="I113" s="1">
-        <f t="shared" si="13"/>
-        <v>400</v>
-      </c>
-      <c r="J113" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K113" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11">
-      <c r="A114" s="80">
-        <v>113</v>
-      </c>
-      <c r="B114" s="100">
-        <v>190</v>
-      </c>
-      <c r="C114" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D114" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E114" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H114" s="1">
-        <v>40</v>
-      </c>
-      <c r="I114" s="1">
-        <f t="shared" si="13"/>
-        <v>400</v>
-      </c>
-      <c r="J114" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K114" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11">
-      <c r="A115" s="80">
-        <v>114</v>
-      </c>
-      <c r="B115" s="100">
-        <v>190</v>
-      </c>
-      <c r="C115" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D115" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E115" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H115" s="1">
-        <v>40</v>
-      </c>
-      <c r="I115" s="1">
-        <f t="shared" si="13"/>
-        <v>400</v>
-      </c>
-      <c r="J115" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K115" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11">
-      <c r="A116" s="80">
-        <v>115</v>
-      </c>
-      <c r="B116" s="100">
-        <v>190</v>
-      </c>
-      <c r="C116" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D116" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E116" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H116" s="1">
-        <v>40</v>
-      </c>
-      <c r="I116" s="1">
-        <f>H116*10</f>
-        <v>400</v>
-      </c>
-      <c r="J116" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K116" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11">
-      <c r="A117" s="80">
-        <v>116</v>
-      </c>
-      <c r="B117" s="100">
-        <v>190</v>
-      </c>
-      <c r="C117" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D117" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E117" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H117" s="1">
-        <v>40</v>
-      </c>
-      <c r="I117" s="1">
-        <f t="shared" ref="I117:I131" si="15">H117*10</f>
-        <v>400</v>
-      </c>
-      <c r="J117" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K117" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11">
-      <c r="A118" s="80">
-        <v>117</v>
-      </c>
-      <c r="B118" s="100">
-        <v>190</v>
-      </c>
-      <c r="C118" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D118" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E118" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H118" s="1">
-        <v>40</v>
-      </c>
-      <c r="I118" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J118" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K118" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11">
-      <c r="A119" s="80">
-        <v>118</v>
-      </c>
-      <c r="B119" s="100">
-        <v>190</v>
-      </c>
-      <c r="C119" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D119" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E119" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H119" s="1">
-        <v>40</v>
-      </c>
-      <c r="I119" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J119" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K119" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11">
-      <c r="A120" s="80">
-        <v>119</v>
-      </c>
-      <c r="B120" s="100">
-        <v>190</v>
-      </c>
-      <c r="C120" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D120" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E120" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H120" s="1">
-        <v>40</v>
-      </c>
-      <c r="I120" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J120" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K120" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11">
-      <c r="A121" s="80">
-        <v>120</v>
-      </c>
-      <c r="B121" s="100">
-        <v>190</v>
-      </c>
-      <c r="C121" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D121" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E121" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H121" s="1">
-        <v>40</v>
-      </c>
-      <c r="I121" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J121" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K121" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11">
-      <c r="A122" s="80">
-        <v>121</v>
-      </c>
-      <c r="B122" s="100">
-        <v>190</v>
-      </c>
-      <c r="C122" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D122" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E122" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F122" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H122" s="1">
-        <v>40</v>
-      </c>
-      <c r="I122" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J122" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K122" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11">
-      <c r="A123" s="80">
-        <v>122</v>
-      </c>
-      <c r="B123" s="100">
-        <v>190</v>
-      </c>
-      <c r="C123" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D123" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E123" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F123" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H123" s="1">
-        <v>40</v>
-      </c>
-      <c r="I123" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J123" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K123" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11">
-      <c r="A124" s="80">
-        <v>123</v>
-      </c>
-      <c r="B124" s="100">
-        <v>190</v>
-      </c>
-      <c r="C124" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D124" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E124" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F124" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G124" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H124" s="1">
-        <v>40</v>
-      </c>
-      <c r="I124" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J124" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K124" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11">
-      <c r="A125" s="80">
-        <v>124</v>
-      </c>
-      <c r="B125" s="100">
-        <v>190</v>
-      </c>
-      <c r="C125" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D125" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E125" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F125" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H125" s="1">
-        <v>40</v>
-      </c>
-      <c r="I125" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J125" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K125" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11">
-      <c r="A126" s="80">
-        <v>125</v>
-      </c>
-      <c r="B126" s="100">
-        <v>190</v>
-      </c>
-      <c r="C126" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D126" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E126" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F126" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H126" s="1">
-        <v>40</v>
-      </c>
-      <c r="I126" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J126" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K126" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11">
-      <c r="A127" s="80">
-        <v>126</v>
-      </c>
-      <c r="B127" s="100">
-        <v>190</v>
-      </c>
-      <c r="C127" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D127" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E127" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F127" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H127" s="1">
-        <v>40</v>
-      </c>
-      <c r="I127" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J127" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K127" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11">
-      <c r="A128" s="80">
-        <v>127</v>
-      </c>
-      <c r="B128" s="100">
-        <v>190</v>
-      </c>
-      <c r="C128" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D128" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E128" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F128" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H128" s="1">
-        <v>40</v>
-      </c>
-      <c r="I128" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J128" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K128" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11">
-      <c r="A129" s="80">
-        <v>128</v>
-      </c>
-      <c r="B129" s="100">
-        <v>190</v>
-      </c>
-      <c r="C129" s="100">
-        <v>11000</v>
-      </c>
-      <c r="D129" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E129" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F129" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H129" s="1">
-        <v>40</v>
-      </c>
-      <c r="I129" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J129" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K129" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" ht="15" customHeight="1">
-      <c r="A130" s="80">
-        <v>129</v>
-      </c>
-      <c r="B130" s="100">
-        <v>190</v>
-      </c>
-      <c r="C130" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D130" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E130" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G130" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H130" s="1">
-        <v>40</v>
-      </c>
-      <c r="I130" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J130" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K130" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" ht="15" customHeight="1">
-      <c r="A131" s="80">
-        <v>130</v>
-      </c>
-      <c r="B131" s="100">
-        <v>190</v>
-      </c>
-      <c r="C131" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D131" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E131" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G131" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H131" s="1">
-        <v>40</v>
-      </c>
-      <c r="I131" s="1">
-        <f t="shared" si="15"/>
-        <v>400</v>
-      </c>
-      <c r="J131" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K131" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" ht="15" customHeight="1">
-      <c r="A132" s="80">
-        <v>131</v>
-      </c>
-      <c r="B132" s="100">
-        <v>190</v>
-      </c>
-      <c r="C132" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D132" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E132" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H132" s="1">
-        <v>40</v>
-      </c>
-      <c r="I132" s="1">
-        <f>H132*10</f>
-        <v>400</v>
-      </c>
-      <c r="J132" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K132" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" ht="15" customHeight="1">
-      <c r="A133" s="80">
-        <v>132</v>
-      </c>
-      <c r="B133" s="100">
-        <v>190</v>
-      </c>
-      <c r="C133" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D133" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E133" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H133" s="1">
-        <v>40</v>
-      </c>
-      <c r="I133" s="1">
-        <f t="shared" ref="I133:I147" si="16">H133*10</f>
-        <v>400</v>
-      </c>
-      <c r="J133" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K133" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" ht="15" customHeight="1">
-      <c r="A134" s="80">
-        <v>133</v>
-      </c>
-      <c r="B134" s="100">
-        <v>190</v>
-      </c>
-      <c r="C134" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D134" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E134" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H134" s="1">
-        <v>40</v>
-      </c>
-      <c r="I134" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J134" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K134" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" ht="15" customHeight="1">
-      <c r="A135" s="80">
-        <v>134</v>
-      </c>
-      <c r="B135" s="100">
-        <v>190</v>
-      </c>
-      <c r="C135" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D135" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E135" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H135" s="1">
-        <v>40</v>
-      </c>
-      <c r="I135" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J135" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K135" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" ht="15" customHeight="1">
-      <c r="A136" s="80">
-        <v>135</v>
-      </c>
-      <c r="B136" s="100">
-        <v>190</v>
-      </c>
-      <c r="C136" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D136" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E136" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H136" s="1">
-        <v>40</v>
-      </c>
-      <c r="I136" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J136" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K136" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" ht="15" customHeight="1">
-      <c r="A137" s="80">
-        <v>136</v>
-      </c>
-      <c r="B137" s="100">
-        <v>190</v>
-      </c>
-      <c r="C137" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D137" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E137" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H137" s="1">
-        <v>40</v>
-      </c>
-      <c r="I137" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J137" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K137" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" ht="15" customHeight="1">
-      <c r="A138" s="80">
-        <v>137</v>
-      </c>
-      <c r="B138" s="100">
-        <v>190</v>
-      </c>
-      <c r="C138" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D138" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E138" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F138" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H138" s="1">
-        <v>40</v>
-      </c>
-      <c r="I138" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J138" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K138" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" ht="15" customHeight="1">
-      <c r="A139" s="80">
-        <v>138</v>
-      </c>
-      <c r="B139" s="100">
-        <v>190</v>
-      </c>
-      <c r="C139" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D139" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E139" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F139" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H139" s="1">
-        <v>40</v>
-      </c>
-      <c r="I139" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J139" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K139" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" ht="15" customHeight="1">
-      <c r="A140" s="80">
-        <v>139</v>
-      </c>
-      <c r="B140" s="100">
-        <v>190</v>
-      </c>
-      <c r="C140" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D140" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E140" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F140" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H140" s="1">
-        <v>40</v>
-      </c>
-      <c r="I140" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J140" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K140" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" ht="15" customHeight="1">
-      <c r="A141" s="80">
-        <v>140</v>
-      </c>
-      <c r="B141" s="100">
-        <v>190</v>
-      </c>
-      <c r="C141" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D141" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E141" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F141" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H141" s="1">
-        <v>40</v>
-      </c>
-      <c r="I141" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J141" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K141" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" ht="15" customHeight="1">
-      <c r="A142" s="80">
-        <v>141</v>
-      </c>
-      <c r="B142" s="100">
-        <v>190</v>
-      </c>
-      <c r="C142" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D142" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E142" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F142" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G142" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H142" s="1">
-        <v>40</v>
-      </c>
-      <c r="I142" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J142" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K142" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" ht="15" customHeight="1">
-      <c r="A143" s="80">
-        <v>142</v>
-      </c>
-      <c r="B143" s="100">
-        <v>190</v>
-      </c>
-      <c r="C143" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D143" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E143" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F143" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H143" s="1">
-        <v>40</v>
-      </c>
-      <c r="I143" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J143" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K143" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" ht="15" customHeight="1">
-      <c r="A144" s="80">
-        <v>143</v>
-      </c>
-      <c r="B144" s="100">
-        <v>190</v>
-      </c>
-      <c r="C144" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D144" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E144" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F144" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G144" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H144" s="1">
-        <v>40</v>
-      </c>
-      <c r="I144" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J144" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K144" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" ht="15" customHeight="1">
-      <c r="A145" s="80">
-        <v>144</v>
-      </c>
-      <c r="B145" s="100">
-        <v>190</v>
-      </c>
-      <c r="C145" s="100">
-        <v>12000</v>
-      </c>
-      <c r="D145" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E145" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F145" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H145" s="1">
-        <v>40</v>
-      </c>
-      <c r="I145" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J145" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K145" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" ht="15" customHeight="1">
-      <c r="A146" s="80">
-        <v>145</v>
-      </c>
-      <c r="B146" s="100">
-        <v>190</v>
-      </c>
-      <c r="C146" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D146" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E146" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H146" s="1">
-        <v>40</v>
-      </c>
-      <c r="I146" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J146" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K146" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" ht="15" customHeight="1">
-      <c r="A147" s="80">
-        <v>146</v>
-      </c>
-      <c r="B147" s="100">
-        <v>190</v>
-      </c>
-      <c r="C147" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D147" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E147" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H147" s="1">
-        <v>40</v>
-      </c>
-      <c r="I147" s="1">
-        <f t="shared" si="16"/>
-        <v>400</v>
-      </c>
-      <c r="J147" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K147" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11" ht="15" customHeight="1">
-      <c r="A148" s="80">
-        <v>147</v>
-      </c>
-      <c r="B148" s="100">
-        <v>190</v>
-      </c>
-      <c r="C148" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D148" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E148" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G148" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H148" s="1">
-        <v>40</v>
-      </c>
-      <c r="I148" s="1">
-        <f>H148*10</f>
-        <v>400</v>
-      </c>
-      <c r="J148" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K148" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11" ht="15" customHeight="1">
-      <c r="A149" s="80">
-        <v>148</v>
-      </c>
-      <c r="B149" s="100">
-        <v>190</v>
-      </c>
-      <c r="C149" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D149" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="E149" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F149" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H149" s="1">
-        <v>40</v>
-      </c>
-      <c r="I149" s="1">
-        <f t="shared" ref="I149:I161" si="17">H149*10</f>
-        <v>400</v>
-      </c>
-      <c r="J149" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K149" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" ht="15" customHeight="1">
-      <c r="A150" s="80">
-        <v>149</v>
-      </c>
-      <c r="B150" s="100">
-        <v>190</v>
-      </c>
-      <c r="C150" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D150" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E150" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G150" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H150" s="1">
-        <v>40</v>
-      </c>
-      <c r="I150" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J150" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K150" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" ht="15" customHeight="1">
-      <c r="A151" s="80">
-        <v>150</v>
-      </c>
-      <c r="B151" s="100">
-        <v>190</v>
-      </c>
-      <c r="C151" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D151" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E151" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G151" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H151" s="1">
-        <v>40</v>
-      </c>
-      <c r="I151" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J151" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K151" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" ht="15" customHeight="1">
-      <c r="A152" s="80">
-        <v>151</v>
-      </c>
-      <c r="B152" s="100">
-        <v>190</v>
-      </c>
-      <c r="C152" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D152" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E152" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G152" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H152" s="1">
-        <v>40</v>
-      </c>
-      <c r="I152" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J152" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K152" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" ht="15" customHeight="1">
-      <c r="A153" s="80">
-        <v>152</v>
-      </c>
-      <c r="B153" s="100">
-        <v>190</v>
-      </c>
-      <c r="C153" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D153" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E153" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H153" s="1">
-        <v>40</v>
-      </c>
-      <c r="I153" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J153" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K153" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" ht="15" customHeight="1">
-      <c r="A154" s="80">
-        <v>153</v>
-      </c>
-      <c r="B154" s="100">
-        <v>190</v>
-      </c>
-      <c r="C154" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D154" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E154" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F154" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G154" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H154" s="1">
-        <v>40</v>
-      </c>
-      <c r="I154" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J154" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K154" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11" ht="15" customHeight="1">
-      <c r="A155" s="80">
-        <v>154</v>
-      </c>
-      <c r="B155" s="100">
-        <v>190</v>
-      </c>
-      <c r="C155" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D155" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E155" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F155" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H155" s="1">
-        <v>40</v>
-      </c>
-      <c r="I155" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J155" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K155" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" ht="15" customHeight="1">
-      <c r="A156" s="80">
-        <v>155</v>
-      </c>
-      <c r="B156" s="100">
-        <v>190</v>
-      </c>
-      <c r="C156" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D156" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E156" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F156" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G156" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H156" s="1">
-        <v>40</v>
-      </c>
-      <c r="I156" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J156" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K156" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11" ht="15" customHeight="1">
-      <c r="A157" s="80">
-        <v>156</v>
-      </c>
-      <c r="B157" s="100">
-        <v>190</v>
-      </c>
-      <c r="C157" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D157" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="E157" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F157" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G157" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H157" s="1">
-        <v>40</v>
-      </c>
-      <c r="I157" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J157" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K157" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11" ht="15" customHeight="1">
-      <c r="A158" s="80">
-        <v>157</v>
-      </c>
-      <c r="B158" s="100">
-        <v>190</v>
-      </c>
-      <c r="C158" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D158" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E158" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F158" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H158" s="1">
-        <v>40</v>
-      </c>
-      <c r="I158" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J158" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K158" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="159" spans="1:11" ht="15" customHeight="1">
-      <c r="A159" s="80">
-        <v>158</v>
-      </c>
-      <c r="B159" s="100">
-        <v>190</v>
-      </c>
-      <c r="C159" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D159" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E159" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F159" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="G159" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H159" s="1">
-        <v>40</v>
-      </c>
-      <c r="I159" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J159" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K159" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="160" spans="1:11" ht="15" customHeight="1">
-      <c r="A160" s="80">
-        <v>159</v>
-      </c>
-      <c r="B160" s="100">
-        <v>190</v>
-      </c>
-      <c r="C160" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D160" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E160" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F160" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H160" s="1">
-        <v>40</v>
-      </c>
-      <c r="I160" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J160" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K160" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="161" spans="1:11" ht="15" customHeight="1">
-      <c r="A161" s="80">
-        <v>160</v>
-      </c>
-      <c r="B161" s="100">
-        <v>190</v>
-      </c>
-      <c r="C161" s="100">
-        <v>13000</v>
-      </c>
-      <c r="D161" s="100" t="s">
-        <v>203</v>
-      </c>
-      <c r="E161" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="F161" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H161" s="1">
-        <v>40</v>
-      </c>
-      <c r="I161" s="1">
-        <f t="shared" si="17"/>
-        <v>400</v>
-      </c>
-      <c r="J161" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K161" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="162" spans="1:11">
-      <c r="A162" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B162" s="99" t="s">
-        <v>18</v>
-      </c>
-      <c r="C162" s="99" t="s">
-        <v>18</v>
-      </c>
-      <c r="D162" s="99" t="s">
-        <v>18</v>
-      </c>
-      <c r="E162" s="99" t="s">
-        <v>18</v>
-      </c>
-      <c r="F162" s="99" t="s">
-        <v>18</v>
-      </c>
-      <c r="G162" s="99" t="s">
-        <v>18</v>
-      </c>
-      <c r="H162" s="99">
-        <f>SUM(H2:H161)</f>
-        <v>6400</v>
-      </c>
-      <c r="I162" s="1">
-        <f>SUM(I2:I161)</f>
-        <v>64000</v>
-      </c>
-      <c r="J162" s="1">
-        <f>COUNTIF(J2:J161,"fft*")</f>
+        <f>SUM(I2:I109)</f>
+        <v>43200</v>
+      </c>
+      <c r="J110" s="1">
+        <f>COUNTIF(J2:J109,"fft*")</f>
         <v>100</v>
       </c>
-      <c r="K162" s="1"/>
+      <c r="K110" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -68373,8 +66501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9383A25-0F16-46DD-90D6-054193614933}">
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74:H81"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="L82" sqref="L82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -70458,7 +68586,7 @@
         <v>250</v>
       </c>
       <c r="H67" s="90" t="str">
-        <f t="shared" ref="H67:H74" si="10">_xlfn.CONCAT("fft_",A67,"_",".txt")</f>
+        <f t="shared" ref="H67:H73" si="10">_xlfn.CONCAT("fft_",A67,"_",".txt")</f>
         <v>fft_66_.txt</v>
       </c>
       <c r="I67" s="80" t="s">
@@ -70915,7 +69043,7 @@
         <v>400</v>
       </c>
       <c r="H82" s="90" t="str">
-        <f t="shared" ref="H76:H105" si="13">_xlfn.CONCAT("fft_",A82,"_",".txt")</f>
+        <f t="shared" ref="H82:H105" si="13">_xlfn.CONCAT("fft_",A82,"_",".txt")</f>
         <v>fft_81_.txt</v>
       </c>
       <c r="I82" s="80" t="s">
@@ -72413,7 +70541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2459949-47C2-499E-B299-8B154CE53211}">
   <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -72479,7 +70607,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E2" s="93" t="s">
         <v>18</v>
@@ -72516,7 +70644,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E3" s="93" t="s">
         <v>18</v>
@@ -72553,7 +70681,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E4" s="93" t="s">
         <v>18</v>
@@ -72590,7 +70718,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" s="93" t="s">
         <v>18</v>
@@ -72627,7 +70755,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E6" s="93" t="s">
         <v>18</v>
@@ -72664,7 +70792,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E7" s="93" t="s">
         <v>18</v>
@@ -72701,7 +70829,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E8" s="93" t="s">
         <v>18</v>
@@ -72738,7 +70866,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E9" s="93" t="s">
         <v>18</v>
@@ -72775,7 +70903,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E10" s="93" t="s">
         <v>18</v>
@@ -72812,7 +70940,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E11" s="93" t="s">
         <v>18</v>
@@ -72849,7 +70977,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E12" s="93" t="s">
         <v>18</v>
@@ -72886,7 +71014,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E13" s="93" t="s">
         <v>18</v>
@@ -72923,7 +71051,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E14" s="93" t="s">
         <v>18</v>
@@ -72960,7 +71088,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E15" s="93" t="s">
         <v>18</v>
@@ -72997,7 +71125,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E16" s="93" t="s">
         <v>18</v>
@@ -73034,7 +71162,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E17" s="93" t="s">
         <v>18</v>
@@ -73071,7 +71199,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E18" s="93" t="s">
         <v>18</v>
@@ -73108,7 +71236,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E19" s="93" t="s">
         <v>18</v>
@@ -73145,7 +71273,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E20" s="93" t="s">
         <v>18</v>
@@ -73182,7 +71310,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E21" s="93" t="s">
         <v>18</v>
@@ -73219,7 +71347,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E22" s="93" t="s">
         <v>18</v>
@@ -73256,7 +71384,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E23" s="93" t="s">
         <v>18</v>
@@ -73293,7 +71421,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E24" s="93" t="s">
         <v>20</v>
@@ -73330,7 +71458,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E25" s="93" t="s">
         <v>20</v>
@@ -73367,7 +71495,7 @@
         <v>5</v>
       </c>
       <c r="D26" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E26" s="93" t="s">
         <v>20</v>
@@ -73404,7 +71532,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E27" s="93" t="s">
         <v>20</v>
@@ -73441,7 +71569,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E28" s="93" t="s">
         <v>20</v>
@@ -73478,7 +71606,7 @@
         <v>5</v>
       </c>
       <c r="D29" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E29" s="93" t="s">
         <v>20</v>
@@ -73515,7 +71643,7 @@
         <v>5</v>
       </c>
       <c r="D30" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E30" s="93" t="s">
         <v>20</v>
@@ -73552,7 +71680,7 @@
         <v>5</v>
       </c>
       <c r="D31" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E31" s="93" t="s">
         <v>20</v>
@@ -73589,7 +71717,7 @@
         <v>5</v>
       </c>
       <c r="D32" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E32" s="93" t="s">
         <v>20</v>
@@ -73626,7 +71754,7 @@
         <v>5</v>
       </c>
       <c r="D33" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E33" s="93" t="s">
         <v>20</v>
@@ -73663,7 +71791,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E34" s="93" t="s">
         <v>20</v>
@@ -73700,7 +71828,7 @@
         <v>5</v>
       </c>
       <c r="D35" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E35" s="93" t="s">
         <v>20</v>
@@ -73737,7 +71865,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E36" s="93" t="s">
         <v>20</v>
@@ -73774,7 +71902,7 @@
         <v>5</v>
       </c>
       <c r="D37" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E37" s="93" t="s">
         <v>20</v>
@@ -73811,7 +71939,7 @@
         <v>5</v>
       </c>
       <c r="D38" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E38" s="93" t="s">
         <v>20</v>
@@ -73848,7 +71976,7 @@
         <v>5</v>
       </c>
       <c r="D39" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E39" s="93" t="s">
         <v>20</v>
@@ -73885,7 +72013,7 @@
         <v>5</v>
       </c>
       <c r="D40" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E40" s="93" t="s">
         <v>20</v>
@@ -73922,7 +72050,7 @@
         <v>5</v>
       </c>
       <c r="D41" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E41" s="93" t="s">
         <v>20</v>
@@ -73959,7 +72087,7 @@
         <v>5</v>
       </c>
       <c r="D42" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E42" s="93" t="s">
         <v>20</v>
@@ -73996,7 +72124,7 @@
         <v>5</v>
       </c>
       <c r="D43" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E43" s="93" t="s">
         <v>20</v>
@@ -74033,7 +72161,7 @@
         <v>5</v>
       </c>
       <c r="D44" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E44" s="93" t="s">
         <v>20</v>
@@ -74070,7 +72198,7 @@
         <v>5</v>
       </c>
       <c r="D45" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E45" s="93" t="s">
         <v>20</v>
@@ -74107,7 +72235,7 @@
         <v>5</v>
       </c>
       <c r="D46" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E46" s="93" t="s">
         <v>20</v>
@@ -74144,7 +72272,7 @@
         <v>5</v>
       </c>
       <c r="D47" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E47" s="93" t="s">
         <v>20</v>
@@ -74181,7 +72309,7 @@
         <v>5</v>
       </c>
       <c r="D48" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E48" s="93" t="s">
         <v>20</v>
@@ -74218,7 +72346,7 @@
         <v>5</v>
       </c>
       <c r="D49" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E49" s="93" t="s">
         <v>20</v>
@@ -74255,7 +72383,7 @@
         <v>5</v>
       </c>
       <c r="D50" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E50" s="93" t="s">
         <v>20</v>
@@ -74292,7 +72420,7 @@
         <v>5</v>
       </c>
       <c r="D51" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E51" s="93" t="s">
         <v>20</v>
@@ -74329,7 +72457,7 @@
         <v>5</v>
       </c>
       <c r="D52" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E52" s="93" t="s">
         <v>20</v>
@@ -74366,7 +72494,7 @@
         <v>5</v>
       </c>
       <c r="D53" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E53" s="93" t="s">
         <v>20</v>
@@ -74403,7 +72531,7 @@
         <v>5</v>
       </c>
       <c r="D54" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E54" s="93" t="s">
         <v>20</v>
@@ -74440,7 +72568,7 @@
         <v>5</v>
       </c>
       <c r="D55" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E55" s="93" t="s">
         <v>20</v>
@@ -74477,7 +72605,7 @@
         <v>5</v>
       </c>
       <c r="D56" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E56" s="93" t="s">
         <v>20</v>
@@ -74514,7 +72642,7 @@
         <v>5</v>
       </c>
       <c r="D57" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E57" s="93" t="s">
         <v>20</v>
@@ -74551,7 +72679,7 @@
         <v>5</v>
       </c>
       <c r="D58" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E58" s="93" t="s">
         <v>20</v>
@@ -74588,7 +72716,7 @@
         <v>5</v>
       </c>
       <c r="D59" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E59" s="93" t="s">
         <v>20</v>
@@ -74625,7 +72753,7 @@
         <v>5</v>
       </c>
       <c r="D60" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E60" s="93" t="s">
         <v>20</v>
@@ -74662,7 +72790,7 @@
         <v>5</v>
       </c>
       <c r="D61" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E61" s="93" t="s">
         <v>20</v>
@@ -74699,7 +72827,7 @@
         <v>5</v>
       </c>
       <c r="D62" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E62" s="93" t="s">
         <v>20</v>
@@ -74736,7 +72864,7 @@
         <v>5</v>
       </c>
       <c r="D63" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E63" s="93" t="s">
         <v>20</v>
@@ -74773,7 +72901,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E64" s="93" t="s">
         <v>20</v>
@@ -74810,7 +72938,7 @@
         <v>5</v>
       </c>
       <c r="D65" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E65" s="93" t="s">
         <v>20</v>
@@ -74847,7 +72975,7 @@
         <v>5</v>
       </c>
       <c r="D66" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E66" s="93" t="s">
         <v>19</v>
@@ -74884,7 +73012,7 @@
         <v>5</v>
       </c>
       <c r="D67" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E67" s="93" t="s">
         <v>19</v>
@@ -74921,7 +73049,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E68" s="93" t="s">
         <v>19</v>
@@ -74958,7 +73086,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E69" s="93" t="s">
         <v>19</v>
@@ -74995,7 +73123,7 @@
         <v>5</v>
       </c>
       <c r="D70" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E70" s="93" t="s">
         <v>19</v>
@@ -75032,7 +73160,7 @@
         <v>5</v>
       </c>
       <c r="D71" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E71" s="93" t="s">
         <v>19</v>
@@ -75069,7 +73197,7 @@
         <v>5</v>
       </c>
       <c r="D72" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E72" s="93" t="s">
         <v>19</v>
@@ -75106,7 +73234,7 @@
         <v>5</v>
       </c>
       <c r="D73" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E73" s="93" t="s">
         <v>19</v>
@@ -75143,7 +73271,7 @@
         <v>5</v>
       </c>
       <c r="D74" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E74" s="93" t="s">
         <v>19</v>
@@ -75180,7 +73308,7 @@
         <v>5</v>
       </c>
       <c r="D75" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E75" s="93" t="s">
         <v>19</v>
@@ -75217,7 +73345,7 @@
         <v>5</v>
       </c>
       <c r="D76" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E76" s="93" t="s">
         <v>19</v>
@@ -75254,7 +73382,7 @@
         <v>5</v>
       </c>
       <c r="D77" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E77" s="93" t="s">
         <v>19</v>
@@ -75291,7 +73419,7 @@
         <v>5</v>
       </c>
       <c r="D78" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E78" s="93" t="s">
         <v>19</v>
@@ -75328,7 +73456,7 @@
         <v>5</v>
       </c>
       <c r="D79" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E79" s="93" t="s">
         <v>19</v>
@@ -75365,7 +73493,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E80" s="93" t="s">
         <v>19</v>
@@ -75402,7 +73530,7 @@
         <v>5</v>
       </c>
       <c r="D81" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E81" s="93" t="s">
         <v>19</v>
@@ -75439,7 +73567,7 @@
         <v>5</v>
       </c>
       <c r="D82" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E82" s="93" t="s">
         <v>19</v>
@@ -75476,7 +73604,7 @@
         <v>5</v>
       </c>
       <c r="D83" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E83" s="93" t="s">
         <v>19</v>
@@ -75513,7 +73641,7 @@
         <v>5</v>
       </c>
       <c r="D84" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E84" s="93" t="s">
         <v>19</v>
@@ -75550,7 +73678,7 @@
         <v>5</v>
       </c>
       <c r="D85" s="93" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E85" s="93" t="s">
         <v>19</v>

</xml_diff>